<commit_message>
added choice of categories to dropdown list
</commit_message>
<xml_diff>
--- a/Zacks_Flask_File/100_SAMPLES.xlsx
+++ b/Zacks_Flask_File/100_SAMPLES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atsukosakurai/Data_Science_Project/Zacks_Flask_File/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BF87CC7-D52C-1D47-8488-14858D5F343A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F485C9D9-3907-F845-BD92-A2C0C98239B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{77BDD069-8AB5-7A41-AE0A-6EC0E51363DC}"/>
   </bookViews>
@@ -756,7 +756,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8FCF987-E434-7647-8F0F-BBC2B07F3C7B}">
   <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>

</xml_diff>